<commit_message>
Başlangıç verilerinin oluşturulması tamamlandı, identity ve token yapısı geliştirilmeye başlandı.
</commit_message>
<xml_diff>
--- a/Surgicalogic.Api/App_Data/Migration/InitialData.xlsx
+++ b/Surgicalogic.Api/App_Data/Migration/InitialData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Meta" sheetId="9" state="hidden" r:id="rId1"/>
+    <sheet name="Meta" sheetId="9" r:id="rId1"/>
     <sheet name="Ekipman Tipi" sheetId="2" r:id="rId2"/>
     <sheet name="Çalışma Tipi" sheetId="1" r:id="rId3"/>
-    <sheet name="Şube" sheetId="5" r:id="rId4"/>
+    <sheet name="Branş" sheetId="5" r:id="rId4"/>
     <sheet name="Ekipman" sheetId="4" r:id="rId5"/>
     <sheet name="Personel Ünvanları" sheetId="6" r:id="rId6"/>
     <sheet name="Personel" sheetId="7" r:id="rId7"/>
@@ -121,7 +121,7 @@
     <t>Ameliyathane</t>
   </si>
   <si>
-    <t>Şube</t>
+    <t>Branş</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>